<commit_message>
updated CDC data 8 APr
</commit_message>
<xml_diff>
--- a/data/CDC_data LARGE.xlsx
+++ b/data/CDC_data LARGE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886589A8-B25F-4BC2-88D7-98E66F11ABD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AE73BE-270F-42AC-8D01-F0277F07D554}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="-30" windowWidth="14955" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="240" windowWidth="14955" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDC_data_as_of_14_Mar" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>6 apr cases</t>
+  </si>
+  <si>
+    <t>7 apr cases</t>
+  </si>
+  <si>
+    <t>25 mar a data</t>
   </si>
 </sst>
 </file>
@@ -931,18 +937,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S87"/>
+  <dimension ref="A1:T88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -971,7 +975,7 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -997,8 +1001,11 @@
       <c r="S1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43842</v>
       </c>
@@ -1053,8 +1060,11 @@
       <c r="S2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43843</v>
       </c>
@@ -1109,8 +1119,11 @@
       <c r="S3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43844</v>
       </c>
@@ -1165,8 +1178,11 @@
       <c r="S4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43845</v>
       </c>
@@ -1221,8 +1237,11 @@
       <c r="S5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43846</v>
       </c>
@@ -1277,8 +1296,11 @@
       <c r="S6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43847</v>
       </c>
@@ -1333,8 +1355,11 @@
       <c r="S7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43848</v>
       </c>
@@ -1389,8 +1414,11 @@
       <c r="S8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43849</v>
       </c>
@@ -1445,8 +1473,11 @@
       <c r="S9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43850</v>
       </c>
@@ -1501,8 +1532,11 @@
       <c r="S10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43851</v>
       </c>
@@ -1557,8 +1591,11 @@
       <c r="S11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43852</v>
       </c>
@@ -1613,8 +1650,11 @@
       <c r="S12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43853</v>
       </c>
@@ -1669,8 +1709,11 @@
       <c r="S13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43854</v>
       </c>
@@ -1725,8 +1768,11 @@
       <c r="S14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43855</v>
       </c>
@@ -1781,8 +1827,11 @@
       <c r="S15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43856</v>
       </c>
@@ -1837,8 +1886,11 @@
       <c r="S16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43857</v>
       </c>
@@ -1893,8 +1945,11 @@
       <c r="S17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43858</v>
       </c>
@@ -1949,8 +2004,11 @@
       <c r="S18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43859</v>
       </c>
@@ -2005,8 +2063,11 @@
       <c r="S19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43860</v>
       </c>
@@ -2061,13 +2122,16 @@
       <c r="S20">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43861</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2117,13 +2181,16 @@
       <c r="S21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43862</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2173,8 +2240,11 @@
       <c r="S22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43863</v>
       </c>
@@ -2229,8 +2299,11 @@
       <c r="S23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43864</v>
       </c>
@@ -2285,8 +2358,11 @@
       <c r="S24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43865</v>
       </c>
@@ -2341,8 +2417,11 @@
       <c r="S25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43866</v>
       </c>
@@ -2397,8 +2476,11 @@
       <c r="S26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43867</v>
       </c>
@@ -2453,13 +2535,16 @@
       <c r="S27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43868</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2509,13 +2594,16 @@
       <c r="S28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43869</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -2565,8 +2653,11 @@
       <c r="S29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43870</v>
       </c>
@@ -2621,8 +2712,11 @@
       <c r="S30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43871</v>
       </c>
@@ -2677,13 +2771,16 @@
       <c r="S31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43872</v>
       </c>
       <c r="B32">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2733,8 +2830,11 @@
       <c r="S32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43873</v>
       </c>
@@ -2789,8 +2889,11 @@
       <c r="S33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43874</v>
       </c>
@@ -2845,13 +2948,16 @@
       <c r="S34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43875</v>
       </c>
       <c r="B35">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -2901,8 +3007,11 @@
       <c r="S35">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43876</v>
       </c>
@@ -2957,13 +3066,16 @@
       <c r="S36">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T36">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43877</v>
       </c>
       <c r="B37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -3013,13 +3125,16 @@
       <c r="S37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43878</v>
       </c>
       <c r="B38">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D38">
         <v>5</v>
@@ -3069,8 +3184,11 @@
       <c r="S38">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43879</v>
       </c>
@@ -3125,13 +3243,16 @@
       <c r="S39">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43880</v>
       </c>
       <c r="B40">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D40">
         <v>6</v>
@@ -3181,8 +3302,11 @@
       <c r="S40">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T40">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43881</v>
       </c>
@@ -3237,13 +3361,16 @@
       <c r="S41">
         <v>29</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T41">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43882</v>
       </c>
       <c r="B42">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D42">
         <v>11</v>
@@ -3293,13 +3420,16 @@
       <c r="S42">
         <v>36</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T42">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43883</v>
       </c>
       <c r="B43">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D43">
         <v>14</v>
@@ -3349,13 +3479,16 @@
       <c r="S43">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T43">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43884</v>
       </c>
       <c r="B44">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D44">
         <v>13</v>
@@ -3405,13 +3538,16 @@
       <c r="S44">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T44">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43885</v>
       </c>
       <c r="B45">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D45">
         <v>34</v>
@@ -3461,13 +3597,16 @@
       <c r="S45">
         <v>82</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43886</v>
       </c>
       <c r="B46">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D46">
         <v>16</v>
@@ -3517,13 +3656,16 @@
       <c r="S46">
         <v>59</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T46">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43887</v>
       </c>
       <c r="B47">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D47">
         <v>30</v>
@@ -3573,13 +3715,16 @@
       <c r="S47">
         <v>98</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T47">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43888</v>
       </c>
       <c r="B48">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D48">
         <v>19</v>
@@ -3629,13 +3774,16 @@
       <c r="S48">
         <v>92</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T48">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43889</v>
       </c>
       <c r="B49">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D49">
         <v>40</v>
@@ -3685,13 +3833,16 @@
       <c r="S49">
         <v>152</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T49">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43890</v>
       </c>
       <c r="B50">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D50">
         <v>40</v>
@@ -3741,13 +3892,16 @@
       <c r="S50">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T50">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43891</v>
       </c>
       <c r="B51">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D51">
         <v>53</v>
@@ -3797,13 +3951,16 @@
       <c r="S51">
         <v>307</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T51">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43892</v>
       </c>
       <c r="B52">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D52">
         <v>51</v>
@@ -3853,13 +4010,16 @@
       <c r="S52">
         <v>300</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T52">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43893</v>
       </c>
       <c r="B53">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="D53">
         <v>48</v>
@@ -3909,13 +4069,16 @@
       <c r="S53">
         <v>341</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T53">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43894</v>
       </c>
       <c r="B54">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="D54">
         <v>58</v>
@@ -3965,13 +4128,16 @@
       <c r="S54">
         <v>386</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T54">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43895</v>
       </c>
       <c r="B55">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D55">
         <v>74</v>
@@ -4021,13 +4187,16 @@
       <c r="S55">
         <v>461</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T55">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43896</v>
       </c>
       <c r="B56">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D56">
         <v>43</v>
@@ -4077,13 +4246,16 @@
       <c r="S56">
         <v>583</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T56">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43897</v>
       </c>
       <c r="B57">
-        <v>682</v>
+        <v>687</v>
       </c>
       <c r="D57">
         <v>79</v>
@@ -4133,13 +4305,16 @@
       <c r="S57">
         <v>650</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T57">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43898</v>
       </c>
       <c r="B58">
-        <v>970</v>
+        <v>984</v>
       </c>
       <c r="D58">
         <v>46</v>
@@ -4189,13 +4364,16 @@
       <c r="S58">
         <v>902</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T58">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43899</v>
       </c>
       <c r="B59">
-        <v>1606</v>
+        <v>1599</v>
       </c>
       <c r="D59">
         <v>50</v>
@@ -4245,13 +4423,16 @@
       <c r="S59">
         <v>1487</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T59">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43900</v>
       </c>
       <c r="B60">
-        <v>1758</v>
+        <v>1760</v>
       </c>
       <c r="D60">
         <v>15</v>
@@ -4301,13 +4482,16 @@
       <c r="S60">
         <v>1618</v>
       </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T60">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43901</v>
       </c>
       <c r="B61">
-        <v>2199</v>
+        <v>2193</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -4357,13 +4541,16 @@
       <c r="S61">
         <v>2033</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T61">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43902</v>
       </c>
       <c r="B62">
-        <v>3140</v>
+        <v>3122</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4413,13 +4600,16 @@
       <c r="S62">
         <v>2747</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T62">
+        <v>3140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43903</v>
       </c>
       <c r="B63">
-        <v>4145</v>
+        <v>4123</v>
       </c>
       <c r="E63">
         <v>2</v>
@@ -4466,13 +4656,16 @@
       <c r="S63">
         <v>3623</v>
       </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T63">
+        <v>4145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43904</v>
       </c>
       <c r="B64">
-        <v>4523</v>
+        <v>4552</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -4519,13 +4712,16 @@
       <c r="S64">
         <v>3881</v>
       </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T64">
+        <v>4523</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>43905</v>
       </c>
       <c r="B65">
-        <v>5572</v>
+        <v>5554</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -4572,13 +4768,16 @@
       <c r="S65">
         <v>4698</v>
       </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T65">
+        <v>5572</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>43906</v>
       </c>
       <c r="B66">
-        <v>6802</v>
+        <v>6844</v>
       </c>
       <c r="G66">
         <v>2</v>
@@ -4619,13 +4818,16 @@
       <c r="S66">
         <v>5580</v>
       </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T66">
+        <v>6802</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>43907</v>
       </c>
       <c r="B67">
-        <v>5934</v>
+        <v>6057</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -4666,13 +4868,16 @@
       <c r="S67">
         <v>4995</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T67">
+        <v>5934</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>43908</v>
       </c>
       <c r="B68">
-        <v>5767</v>
+        <v>5886</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -4713,13 +4918,16 @@
       <c r="S68">
         <v>4807</v>
       </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T68">
+        <v>5767</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>43909</v>
       </c>
       <c r="B69">
-        <v>7307</v>
+        <v>7481</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -4757,13 +4965,16 @@
       <c r="S69">
         <v>5548</v>
       </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T69">
+        <v>7307</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>43910</v>
       </c>
       <c r="B70">
-        <v>8043</v>
+        <v>8430</v>
       </c>
       <c r="I70">
         <v>2</v>
@@ -4798,13 +5009,16 @@
       <c r="S70">
         <v>5959</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T70">
+        <v>8043</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>43911</v>
       </c>
       <c r="B71">
-        <v>7862</v>
+        <v>8440</v>
       </c>
       <c r="J71">
         <v>2</v>
@@ -4836,13 +5050,16 @@
       <c r="S71">
         <v>5598</v>
       </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T71">
+        <v>7862</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>43912</v>
       </c>
       <c r="B72">
-        <v>8150</v>
+        <v>8836</v>
       </c>
       <c r="J72">
         <v>1</v>
@@ -4874,13 +5091,16 @@
       <c r="S72">
         <v>5563</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T72">
+        <v>8150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>43913</v>
       </c>
       <c r="B73">
-        <v>8407</v>
+        <v>9529</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -4912,13 +5132,16 @@
       <c r="S73">
         <v>5449</v>
       </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T73">
+        <v>8407</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>43914</v>
       </c>
       <c r="B74">
-        <v>6009</v>
+        <v>6854</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -4947,13 +5170,16 @@
       <c r="S74">
         <v>3744</v>
       </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T74">
+        <v>6009</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>43915</v>
       </c>
       <c r="B75">
-        <v>5320</v>
+        <v>6348</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -4979,13 +5205,16 @@
       <c r="S75">
         <v>3261</v>
       </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T75">
+        <v>5320</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>43916</v>
       </c>
       <c r="B76">
-        <v>8321</v>
+        <v>9965</v>
       </c>
       <c r="M76">
         <v>1</v>
@@ -5008,13 +5237,16 @@
       <c r="S76">
         <v>4314</v>
       </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="T76">
+        <v>8321</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
         <v>43917</v>
       </c>
       <c r="B77">
-        <v>8121</v>
+        <v>9788</v>
       </c>
       <c r="O77">
         <v>10</v>
@@ -5031,13 +5263,16 @@
       <c r="S77">
         <v>3545</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T77">
+        <v>8121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>43918</v>
       </c>
       <c r="B78">
-        <v>7428</v>
+        <v>9378</v>
       </c>
       <c r="O78">
         <v>2</v>
@@ -5054,13 +5289,16 @@
       <c r="S78">
         <v>2959</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T78">
+        <v>7428</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>43919</v>
       </c>
       <c r="B79">
-        <v>6089</v>
+        <v>8738</v>
       </c>
       <c r="O79">
         <v>0</v>
@@ -5077,13 +5315,16 @@
       <c r="S79">
         <v>2066</v>
       </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T79">
+        <v>6089</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>43920</v>
       </c>
       <c r="B80">
-        <v>4219</v>
+        <v>7950</v>
       </c>
       <c r="P80">
         <v>3</v>
@@ -5097,13 +5338,16 @@
       <c r="S80">
         <v>1013</v>
       </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T80">
+        <v>4219</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>43921</v>
       </c>
       <c r="B81">
-        <v>2275</v>
+        <v>4352</v>
       </c>
       <c r="P81">
         <v>0</v>
@@ -5117,13 +5361,16 @@
       <c r="S81">
         <v>394</v>
       </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T81">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>43922</v>
       </c>
       <c r="B82">
-        <v>594</v>
+        <v>2255</v>
       </c>
       <c r="Q82">
         <v>0</v>
@@ -5134,13 +5381,16 @@
       <c r="S82">
         <v>187</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T82">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>43923</v>
       </c>
       <c r="B83">
-        <v>231</v>
+        <v>1185</v>
       </c>
       <c r="R83">
         <v>0</v>
@@ -5148,48 +5398,68 @@
       <c r="S83">
         <v>72</v>
       </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T83">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>43924</v>
       </c>
       <c r="B84">
-        <v>76</v>
+        <v>243</v>
       </c>
       <c r="S84">
         <v>12</v>
       </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T84">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>43925</v>
       </c>
       <c r="B85">
+        <v>132</v>
+      </c>
+      <c r="S85">
+        <v>0</v>
+      </c>
+      <c r="T85">
         <v>28</v>
       </c>
-      <c r="S85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>43926</v>
       </c>
       <c r="B86">
+        <v>47</v>
+      </c>
+      <c r="S86">
+        <v>0</v>
+      </c>
+      <c r="T86">
         <v>5</v>
       </c>
-      <c r="S86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>43927</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="S87">
+        <v>0</v>
+      </c>
+      <c r="T87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B88">
         <v>0</v>
       </c>
     </row>

</xml_diff>